<commit_message>
changed sendNegotiation to send an arbitrary number of nodes
</commit_message>
<xml_diff>
--- a/Communication protocols.xlsx
+++ b/Communication protocols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loure\Dropbox\Lourenço\Faculdade\5A1S\SCDTR\SCDTR-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F340FF66-5D78-4A20-8E25-696FB89CC074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373F6A14-A30E-47A2-B453-B4BC7901517A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,68 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-    <author>Lourenço Vaz Pato</author>
-  </authors>
-  <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Duarte Dias:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">O "1" refere-se ao tipo de mensagem que é
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{37ADC715-1121-4291-B6D6-B92003BEC17C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lourenço Vaz Pato:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Pode não ser preciso mandar esta mensagem. Se o server sabe o estado de ocupação da secretária (messageType=3), pode saber já qual é a referência correspondente para cada secretária</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
   <si>
     <t>Command</t>
   </si>
@@ -398,12 +338,6 @@
     <t>&lt;address&gt; is the address of the sending node &lt;val&gt; is floating point number expressing measured illuminance in lux between 0 and 500.</t>
   </si>
   <si>
-    <t>&lt;address&gt;2&lt;val1&gt;&lt;val2&gt;</t>
-  </si>
-  <si>
-    <t>&lt;val1&gt; is a proposed PWM value for node 1 and &lt;val2&gt; is a proposed PWM value for node2</t>
-  </si>
-  <si>
     <t>Send negotiation message (local solution)</t>
   </si>
   <si>
@@ -443,9 +377,6 @@
     <t>sendNegotiationState(&lt;v&gt;)</t>
   </si>
   <si>
-    <t>sendNegotiation(&lt;v1&gt;,&lt;v2&gt;)</t>
-  </si>
-  <si>
     <t>&lt;val&gt; is floating point number expressing the illuminance PWM control reference (obtained by consensus) between 0 and 5.</t>
   </si>
   <si>
@@ -453,13 +384,25 @@
   </si>
   <si>
     <t>&lt;val&gt; is a Boolean flag: 1 - ready to begin negotiation  0 - not negotiating  -1 - reset system setup</t>
+  </si>
+  <si>
+    <t>sendNegotiation(&lt;v&gt;,N)</t>
+  </si>
+  <si>
+    <t>&lt;add&gt;2&lt;N&gt;&lt;val 1&gt;...&lt;val N&gt;</t>
+  </si>
+  <si>
+    <t>&lt;N&gt; is the number of nodes to be sent &lt;val i&gt; is a proposed PWM value for node i</t>
+  </si>
+  <si>
+    <t>&gt;5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -479,30 +422,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -531,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,6 +473,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -986,11 +913,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -998,7 +925,7 @@
     <col min="1" max="1" width="25.08203125" customWidth="1"/>
     <col min="2" max="2" width="17.9140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.9140625" customWidth="1"/>
     <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="43.58203125" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" customWidth="1"/>
@@ -1028,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -1054,7 +981,7 @@
         <v>80</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1">
         <v>2</v>
@@ -1081,7 +1008,7 @@
         <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -1107,7 +1034,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -1121,19 +1048,19 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E5" s="6">
         <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H5" s="7">
         <v>2</v>
@@ -1156,10 +1083,10 @@
         <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
@@ -1182,10 +1109,10 @@
         <v>4</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H7" s="7">
         <v>2</v>
@@ -1193,19 +1120,19 @@
     </row>
     <row r="8" spans="1:10" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>82</v>
+      <c r="D8" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -1213,19 +1140,19 @@
     </row>
     <row r="9" spans="1:10" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -1429,12 +1356,11 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>